<commit_message>
move files and remove tests
</commit_message>
<xml_diff>
--- a/your-project/3_daily_pollution.xlsx
+++ b/your-project/3_daily_pollution.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cunillet/Desktop/cunillet/module1/Project-Week-2-Barcelona/your-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64A1D4A6-10A9-6844-9FB3-7ACA112FC96F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0D8832-B9CB-A14B-8886-6465E130FD60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{88797791-CB41-B843-B81A-225CFA608290}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{88797791-CB41-B843-B81A-225CFA608290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="62">
   <si>
     <t>AVG of a week</t>
   </si>
@@ -96,13 +97,211 @@
   </si>
   <si>
     <t>AVG Sunday</t>
+  </si>
+  <si>
+    <t>AVG_Hour</t>
+  </si>
+  <si>
+    <t>7h-9h</t>
+  </si>
+  <si>
+    <t>10h-12h</t>
+  </si>
+  <si>
+    <t>13h-15h</t>
+  </si>
+  <si>
+    <t>17h-19h</t>
+  </si>
+  <si>
+    <t>20h-22h</t>
+  </si>
+  <si>
+    <t>Qualitative name</t>
+  </si>
+  <si>
+    <t>Index or sub-index</t>
+  </si>
+  <si>
+    <r>
+      <t>Pollutant (hourly) density in μg/m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PM</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PM</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(optional)</t>
+    </r>
+  </si>
+  <si>
+    <t>Very low</t>
+  </si>
+  <si>
+    <t>0–25</t>
+  </si>
+  <si>
+    <t>0–50</t>
+  </si>
+  <si>
+    <t>0–60</t>
+  </si>
+  <si>
+    <t>0–15</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>25–50</t>
+  </si>
+  <si>
+    <t>50–100</t>
+  </si>
+  <si>
+    <t>60–120</t>
+  </si>
+  <si>
+    <t>15–30</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>50–75</t>
+  </si>
+  <si>
+    <t>100–200</t>
+  </si>
+  <si>
+    <t>50–90</t>
+  </si>
+  <si>
+    <t>120–180</t>
+  </si>
+  <si>
+    <t>30–55</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>75–100</t>
+  </si>
+  <si>
+    <t>200–400</t>
+  </si>
+  <si>
+    <t>90–180</t>
+  </si>
+  <si>
+    <t>180–240</t>
+  </si>
+  <si>
+    <t>55–110</t>
+  </si>
+  <si>
+    <t>Very high</t>
+  </si>
+  <si>
+    <t>&gt;100</t>
+  </si>
+  <si>
+    <t>&gt;400</t>
+  </si>
+  <si>
+    <t>&gt;180</t>
+  </si>
+  <si>
+    <t>&gt;240</t>
+  </si>
+  <si>
+    <t>&gt;110</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,16 +309,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,18 +369,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="9"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -167,11 +470,25 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{1B47ABDB-79CC-AA4E-9F75-C868C192A719}" name="AVG of a week"/>
     <tableColumn id="2" xr3:uid="{82E5BB2C-DC6B-B14A-ABDD-77C39812D9F6}" name="STATION"/>
-    <tableColumn id="3" xr3:uid="{D112640C-CF0E-0543-94C3-0B6D74F4800D}" name="AVG_PM" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{CF2D4C36-EF75-2247-8642-20F470A72237}" name="AVG_O3" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{081B6236-B9E6-944A-8918-4C16B117A1BE}" name="AVG_NO2" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{D112640C-CF0E-0543-94C3-0B6D74F4800D}" name="AVG_PM" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{CF2D4C36-EF75-2247-8642-20F470A72237}" name="AVG_O3" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{081B6236-B9E6-944A-8918-4C16B117A1BE}" name="AVG_NO2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{07E62E36-F31C-DF48-819C-476AA3E224FF}" name="Table2" displayName="Table2" ref="I1:M45" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="I1:M45" xr:uid="{B9338B7F-5562-DE46-861B-4CA53FE6B9F3}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C21991C1-D91E-854F-8DC3-C768D7F625E6}" name="AVG_Hour"/>
+    <tableColumn id="2" xr3:uid="{2AC06000-4B7E-344D-9116-6E2041F5B6B3}" name="STATION"/>
+    <tableColumn id="3" xr3:uid="{8C83AACF-3282-4944-8DA4-34B65AB7857E}" name="AVG_PM" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D58E6AB7-98C2-7944-B802-9C4E4314F282}" name="AVG_O3" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{46B4C0FC-B97B-DE48-8F75-208DC0EBD3DE}" name="AVG_NO2" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -472,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6994680-906B-5844-A21E-5E1F392417EA}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,9 +802,14 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,8 +825,23 @@
       <c r="E1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -517,8 +854,23 @@
       <c r="E2" s="1">
         <v>375926</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <v>300000</v>
+      </c>
+      <c r="M2" s="1">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -531,8 +883,20 @@
       <c r="E3" s="1">
         <v>530876</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>200000</v>
+      </c>
+      <c r="L3" s="1">
+        <v>306667</v>
+      </c>
+      <c r="M3" s="1">
+        <v>286667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -545,8 +909,20 @@
       <c r="E4" s="1">
         <v>444967</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>176667</v>
+      </c>
+      <c r="L4" s="1">
+        <v>240000</v>
+      </c>
+      <c r="M4" s="1">
+        <v>455000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -559,8 +935,20 @@
       <c r="E5" s="1">
         <v>118393</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>90000</v>
+      </c>
+      <c r="L5" s="1">
+        <v>610000</v>
+      </c>
+      <c r="M5" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -573,8 +961,20 @@
       <c r="E6" s="1">
         <v>270655</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>120000</v>
+      </c>
+      <c r="L6" s="1">
+        <v>400000</v>
+      </c>
+      <c r="M6" s="1">
+        <v>156667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -587,8 +987,20 @@
       <c r="E7" s="1">
         <v>413713</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1">
+        <v>196667</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="1">
+        <v>256667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -601,8 +1013,20 @@
       <c r="E8" s="1">
         <v>345597</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="1">
+        <v>206667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -615,8 +1039,20 @@
       <c r="E9" s="1">
         <v>294142</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="1">
+        <v>140000</v>
+      </c>
+      <c r="L9" s="1">
+        <v>363333</v>
+      </c>
+      <c r="M9" s="1">
+        <v>243333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -632,8 +1068,23 @@
       <c r="E11" s="1">
         <v>420500</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>263333</v>
+      </c>
+      <c r="M11" s="1">
+        <v>390000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -646,8 +1097,20 @@
       <c r="E12" s="1">
         <v>496364</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1">
+        <v>200000</v>
+      </c>
+      <c r="L12" s="1">
+        <v>180000</v>
+      </c>
+      <c r="M12" s="1">
+        <v>493333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -660,8 +1123,20 @@
       <c r="E13" s="1">
         <v>522917</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1">
+        <v>170000</v>
+      </c>
+      <c r="L13" s="1">
+        <v>230000</v>
+      </c>
+      <c r="M13" s="1">
+        <v>453333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -674,8 +1149,20 @@
       <c r="E14" s="1">
         <v>143200</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>90000</v>
+      </c>
+      <c r="L14" s="1">
+        <v>570000</v>
+      </c>
+      <c r="M14" s="1">
+        <v>73333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -688,8 +1175,20 @@
       <c r="E15" s="1">
         <v>329167</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="1">
+        <v>120000</v>
+      </c>
+      <c r="L15" s="1">
+        <v>333333</v>
+      </c>
+      <c r="M15" s="1">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -702,8 +1201,20 @@
       <c r="E16" s="1">
         <v>476000</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="1">
+        <v>206667</v>
+      </c>
+      <c r="L16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>426667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -716,8 +1227,20 @@
       <c r="E17" s="1">
         <v>434800</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>373333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -730,8 +1253,20 @@
       <c r="E18" s="1">
         <v>361200</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="1">
+        <v>140000</v>
+      </c>
+      <c r="L18" s="1">
+        <v>383333</v>
+      </c>
+      <c r="M18" s="1">
+        <v>253333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -747,8 +1282,23 @@
       <c r="E20" s="1">
         <v>335000</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <v>380000</v>
+      </c>
+      <c r="M20" s="1">
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -761,8 +1311,20 @@
       <c r="E21" s="1">
         <v>380000</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" s="1">
+        <v>200000</v>
+      </c>
+      <c r="L21" s="1">
+        <v>250000</v>
+      </c>
+      <c r="M21" s="1">
+        <v>440000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -775,8 +1337,20 @@
       <c r="E22" s="1">
         <v>383333</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="1">
+        <v>170000</v>
+      </c>
+      <c r="L22" s="1">
+        <v>360000</v>
+      </c>
+      <c r="M22" s="1">
+        <v>310000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -789,8 +1363,20 @@
       <c r="E23" s="1">
         <v>104000</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23" s="1">
+        <v>90000</v>
+      </c>
+      <c r="L23" s="1">
+        <v>563333</v>
+      </c>
+      <c r="M23" s="1">
+        <v>76667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -803,8 +1389,20 @@
       <c r="E24" s="1">
         <v>208800</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K24" s="1">
+        <v>120000</v>
+      </c>
+      <c r="L24" s="1">
+        <v>413333</v>
+      </c>
+      <c r="M24" s="1">
+        <v>156667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -817,8 +1415,20 @@
       <c r="E25" s="1">
         <v>378400</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="1">
+        <v>220000</v>
+      </c>
+      <c r="L25" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="1">
+        <v>256667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -831,8 +1441,20 @@
       <c r="E26" s="1">
         <v>281200</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="1">
+        <v>196667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -845,8 +1467,20 @@
       <c r="E27" s="1">
         <v>259600</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="1">
+        <v>136667</v>
+      </c>
+      <c r="L27" s="1">
+        <v>470000</v>
+      </c>
+      <c r="M27" s="1">
+        <v>166667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -862,8 +1496,23 @@
       <c r="E29" s="1">
         <v>255200</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="1">
+        <v>330000</v>
+      </c>
+      <c r="M29" s="1">
+        <v>380000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -876,8 +1525,20 @@
       <c r="E30" s="1">
         <v>397083</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="1">
+        <v>183333</v>
+      </c>
+      <c r="L30" s="1">
+        <v>240000</v>
+      </c>
+      <c r="M30" s="1">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>4</v>
       </c>
@@ -890,8 +1551,20 @@
       <c r="E31" s="1">
         <v>260455</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" s="1">
+        <v>150000</v>
+      </c>
+      <c r="L31" s="1">
+        <v>340000</v>
+      </c>
+      <c r="M31" s="1">
+        <v>340000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>5</v>
       </c>
@@ -904,8 +1577,20 @@
       <c r="E32" s="1">
         <v>77500</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" s="1">
+        <v>90000</v>
+      </c>
+      <c r="L32" s="1">
+        <v>513333</v>
+      </c>
+      <c r="M32" s="1">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>6</v>
       </c>
@@ -918,8 +1603,20 @@
       <c r="E33" s="1">
         <v>120000</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K33" s="1">
+        <v>116667</v>
+      </c>
+      <c r="L33" s="1">
+        <v>393333</v>
+      </c>
+      <c r="M33" s="1">
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -932,8 +1629,20 @@
       <c r="E34" s="1">
         <v>309600</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="1">
+        <v>213333</v>
+      </c>
+      <c r="L34" t="s">
+        <v>2</v>
+      </c>
+      <c r="M34" s="1">
+        <v>430000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>8</v>
       </c>
@@ -946,8 +1655,20 @@
       <c r="E35" s="1">
         <v>211600</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" t="s">
+        <v>2</v>
+      </c>
+      <c r="L35" t="s">
+        <v>2</v>
+      </c>
+      <c r="M35" s="1">
+        <v>303333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>9</v>
       </c>
@@ -960,8 +1681,20 @@
       <c r="E36" s="1">
         <v>155600</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" s="1">
+        <v>146667</v>
+      </c>
+      <c r="L36" s="1">
+        <v>400000</v>
+      </c>
+      <c r="M36" s="1">
+        <v>283333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -977,8 +1710,23 @@
       <c r="E38" s="1">
         <v>223600</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L38" s="1">
+        <v>323333</v>
+      </c>
+      <c r="M38" s="1">
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -991,8 +1739,20 @@
       <c r="E39" s="1">
         <v>513333</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>3</v>
+      </c>
+      <c r="K39" s="1">
+        <v>160000</v>
+      </c>
+      <c r="L39" s="1">
+        <v>240000</v>
+      </c>
+      <c r="M39" s="1">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>4</v>
       </c>
@@ -1005,8 +1765,20 @@
       <c r="E40" s="1">
         <v>269000</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="1">
+        <v>136667</v>
+      </c>
+      <c r="L40" s="1">
+        <v>230000</v>
+      </c>
+      <c r="M40" s="1">
+        <v>380000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>5</v>
       </c>
@@ -1019,8 +1791,20 @@
       <c r="E41" s="1">
         <v>64000</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>5</v>
+      </c>
+      <c r="K41" s="1">
+        <v>90000</v>
+      </c>
+      <c r="L41" s="1">
+        <v>413333</v>
+      </c>
+      <c r="M41" s="1">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>6</v>
       </c>
@@ -1033,8 +1817,20 @@
       <c r="E42" s="1">
         <v>127200</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J42" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="1">
+        <v>103333</v>
+      </c>
+      <c r="L42" s="1">
+        <v>363333</v>
+      </c>
+      <c r="M42" s="1">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>7</v>
       </c>
@@ -1047,8 +1843,20 @@
       <c r="E43" s="1">
         <v>284783</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J43" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="1">
+        <v>193333</v>
+      </c>
+      <c r="L43" t="s">
+        <v>2</v>
+      </c>
+      <c r="M43" s="1">
+        <v>453333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>8</v>
       </c>
@@ -1061,8 +1869,20 @@
       <c r="E44" s="1">
         <v>244400</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J44" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" t="s">
+        <v>2</v>
+      </c>
+      <c r="L44" t="s">
+        <v>2</v>
+      </c>
+      <c r="M44" s="1">
+        <v>326667</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>9</v>
       </c>
@@ -1075,8 +1895,20 @@
       <c r="E45" s="1">
         <v>169600</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" s="1">
+        <v>140000</v>
+      </c>
+      <c r="L45" s="1">
+        <v>370000</v>
+      </c>
+      <c r="M45" s="1">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -1093,7 +1925,7 @@
         <v>625600</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>3</v>
       </c>
@@ -1423,8 +2255,151 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3B0132-BD79-8B42-92E2-105064094F2C}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>